<commit_message>
Atualização da planilha de testes
</commit_message>
<xml_diff>
--- a/Data Files/AutoExec_GH - [Template].xlsx
+++ b/Data Files/AutoExec_GH - [Template].xlsx
@@ -24,6 +24,9 @@
   </si>
   <si>
     <t>Select TestCases</t>
+  </si>
+  <si>
+    <t>Configurações gerais</t>
   </si>
   <si>
     <t>Test Case Name</t>
@@ -237,9 +240,6 @@
     <t>O Sistema DEVE exibir uma mensagem indicando que o campo é de preenchimento obrigatório</t>
   </si>
   <si>
-    <t>Configurações gerais</t>
-  </si>
-  <si>
     <t>Path APK</t>
   </si>
   <si>
@@ -249,7 +249,7 @@
     <t>Path Screenshots</t>
   </si>
   <si>
-    <t>Screenshots/</t>
+    <t>Screenshots</t>
   </si>
 </sst>
 </file>
@@ -816,49 +816,49 @@
         <v>0</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E5" s="14" t="s">
         <v>2</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G5" s="15" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H5" s="16" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I5" s="17" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J5" s="14" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="K5" s="18" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="L5" s="19" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="M5" s="20" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="N5" s="20" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="O5" s="20" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="P5" s="20" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="Q5" s="9"/>
       <c r="R5" s="9"/>
@@ -878,16 +878,16 @@
         <v>1</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E6" s="23" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F6" s="24" t="str">
         <f>HYPERLINK("http://docs.mv.com.br/pages/viewpage.action?pageId=15310994","LINK UC")</f>
@@ -897,13 +897,13 @@
         <v>1.0</v>
       </c>
       <c r="H6" s="26" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I6" s="26" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J6" s="27" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K6" s="28"/>
       <c r="L6" s="29" t="str">
@@ -911,16 +911,16 @@
         <v>LINK EVIDÊNCIA</v>
       </c>
       <c r="M6" s="30" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="N6" s="30" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O6" s="30" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="P6" s="31" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7">
@@ -934,25 +934,25 @@
         <v>2.0</v>
       </c>
       <c r="H7" s="35" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I7" s="35" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J7" s="36"/>
       <c r="K7" s="36"/>
       <c r="L7" s="37"/>
       <c r="M7" s="30" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="N7" s="30" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="O7" s="30" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="P7" s="31" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8">
@@ -966,25 +966,25 @@
         <v>3.0</v>
       </c>
       <c r="H8" s="35" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I8" s="35" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J8" s="36"/>
       <c r="K8" s="36"/>
       <c r="L8" s="37"/>
       <c r="M8" s="30" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="N8" s="30">
         <v>6.7628356788E10</v>
       </c>
       <c r="O8" s="30" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="P8" s="31" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9">
@@ -998,25 +998,25 @@
         <v>4.0</v>
       </c>
       <c r="H9" s="35" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I9" s="35" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J9" s="36"/>
       <c r="K9" s="36"/>
       <c r="L9" s="37"/>
       <c r="M9" s="30" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="N9" s="30">
         <v>2.9121986E7</v>
       </c>
       <c r="O9" s="30" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="P9" s="31" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10">
@@ -1030,25 +1030,25 @@
         <v>5.0</v>
       </c>
       <c r="H10" s="35" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="I10" s="35" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J10" s="36"/>
       <c r="K10" s="36"/>
       <c r="L10" s="37"/>
       <c r="M10" s="30" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="N10" s="30" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="O10" s="30" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="P10" s="31" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11">
@@ -1062,25 +1062,25 @@
         <v>6.0</v>
       </c>
       <c r="H11" s="35" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="I11" s="35" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J11" s="36"/>
       <c r="K11" s="36"/>
       <c r="L11" s="37"/>
       <c r="M11" s="30" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="N11" s="30">
         <v>8.1999002918E10</v>
       </c>
       <c r="O11" s="30" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="P11" s="31" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12">
@@ -1091,19 +1091,19 @@
     </row>
     <row r="13">
       <c r="A13" s="40" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B13" s="22" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C13" s="21" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D13" s="23" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E13" s="23" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F13" s="24" t="str">
         <f>HYPERLINK("http://docs.mv.com.br/pages/viewpage.action?pageId=15310994","LINK UC")</f>
@@ -1113,13 +1113,13 @@
         <v>1.0</v>
       </c>
       <c r="H13" s="26" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I13" s="26" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="J13" s="27" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K13" s="28"/>
       <c r="L13" s="29" t="str">
@@ -1127,16 +1127,16 @@
         <v>LINK EVIDÊNCIA</v>
       </c>
       <c r="M13" s="30" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="N13" s="30" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="O13" s="30" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="P13" s="31" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14">
@@ -1150,25 +1150,25 @@
         <v>2.0</v>
       </c>
       <c r="H14" s="35" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="I14" s="35" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="J14" s="36"/>
       <c r="K14" s="36"/>
       <c r="L14" s="37"/>
       <c r="M14" s="30" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="N14" s="30" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="O14" s="30" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="P14" s="31" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15">
@@ -1182,25 +1182,25 @@
         <v>3.0</v>
       </c>
       <c r="H15" s="35" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I15" s="35" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="J15" s="36"/>
       <c r="K15" s="36"/>
       <c r="L15" s="37"/>
       <c r="M15" s="30" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="N15" s="30" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="O15" s="30" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="P15" s="31" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16">
@@ -6839,7 +6839,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="41" t="s">
-        <v>52</v>
+        <v>4</v>
       </c>
       <c r="B1" s="42"/>
       <c r="C1" s="43"/>

</xml_diff>